<commit_message>
feat: Implement PosProxy.Merge, CalculationMode
</commit_message>
<xml_diff>
--- a/src/EasyOpenXml.Excel.DemoConsole/Assets/template.xlsx
+++ b/src/EasyOpenXml.Excel.DemoConsole/Assets/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogawa\github\csharp\EasyOpenXml.Net8\src\EasyOpenXml.Excel.DemoConsole\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73E0361-2308-4E79-B4B3-A00EADD43B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0851D345-E685-4519-A8D5-F006B9503055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="24700" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,11 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -69,8 +68,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,13 +353,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>1</v>
       </c>
@@ -367,7 +365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -375,7 +373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>3</v>
       </c>
@@ -391,12 +389,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFEF49F0-0650-4612-8067-793ACD206277}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -408,7 +427,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -421,7 +440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>